<commit_message>
changed recommendation & app
</commit_message>
<xml_diff>
--- a/data/champ_role.xlsx
+++ b/data/champ_role.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\app lol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\app lol\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB6D4BA-2C98-4F44-9A8B-382F4A88E990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4702D0B0-0546-42A1-BBD5-551FD34451D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="201">
   <si>
     <t>Aatrox</t>
   </si>
@@ -619,6 +619,15 @@
   </si>
   <si>
     <t>Middle,Bottom</t>
+  </si>
+  <si>
+    <t>AD/AP</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>AP</t>
   </si>
 </sst>
 </file>
@@ -788,15 +797,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.140625"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="4.42578125" customWidth="1"/>
@@ -814,6 +823,9 @@
       <c r="B1" t="s">
         <v>195</v>
       </c>
+      <c r="C1" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -822,6 +834,9 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>199</v>
+      </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -831,6 +846,9 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>200</v>
+      </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -840,6 +858,9 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>200</v>
+      </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -849,6 +870,9 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
+      <c r="C5" t="s">
+        <v>199</v>
+      </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -858,6 +882,9 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
+      <c r="C6" t="s">
+        <v>199</v>
+      </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -867,6 +894,9 @@
       <c r="B7" t="s">
         <v>1</v>
       </c>
+      <c r="C7" t="s">
+        <v>199</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -876,6 +906,9 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
+      <c r="C8" t="s">
+        <v>200</v>
+      </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -885,6 +918,9 @@
       <c r="B9" t="s">
         <v>147</v>
       </c>
+      <c r="C9" t="s">
+        <v>200</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -894,6 +930,9 @@
       <c r="B10" t="s">
         <v>3</v>
       </c>
+      <c r="C10" t="s">
+        <v>200</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -903,6 +942,9 @@
       <c r="B11" t="s">
         <v>14</v>
       </c>
+      <c r="C11" t="s">
+        <v>199</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -912,6 +954,9 @@
       <c r="B12" t="s">
         <v>14</v>
       </c>
+      <c r="C12" t="s">
+        <v>199</v>
+      </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -921,6 +966,9 @@
       <c r="B13" t="s">
         <v>3</v>
       </c>
+      <c r="C13" t="s">
+        <v>200</v>
+      </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -930,6 +978,9 @@
       <c r="B14" t="s">
         <v>19</v>
       </c>
+      <c r="C14" t="s">
+        <v>200</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -939,6 +990,9 @@
       <c r="B15" t="s">
         <v>3</v>
       </c>
+      <c r="C15" t="s">
+        <v>200</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -948,6 +1002,9 @@
       <c r="B16" t="s">
         <v>8</v>
       </c>
+      <c r="C16" t="s">
+        <v>200</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -957,6 +1014,9 @@
       <c r="B17" t="s">
         <v>23</v>
       </c>
+      <c r="C17" t="s">
+        <v>199</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -966,6 +1026,9 @@
       <c r="B18" t="s">
         <v>8</v>
       </c>
+      <c r="C18" t="s">
+        <v>199</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -975,6 +1038,9 @@
       <c r="B19" t="s">
         <v>26</v>
       </c>
+      <c r="C19" t="s">
+        <v>200</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -984,6 +1050,9 @@
       <c r="B20" t="s">
         <v>8</v>
       </c>
+      <c r="C20" t="s">
+        <v>199</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -993,6 +1062,9 @@
       <c r="B21" t="s">
         <v>23</v>
       </c>
+      <c r="C21" t="s">
+        <v>199</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1002,6 +1074,9 @@
       <c r="B22" t="s">
         <v>14</v>
       </c>
+      <c r="C22" t="s">
+        <v>199</v>
+      </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1011,6 +1086,9 @@
       <c r="B23" t="s">
         <v>31</v>
       </c>
+      <c r="C23" t="s">
+        <v>199</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1020,6 +1098,9 @@
       <c r="B24" t="s">
         <v>147</v>
       </c>
+      <c r="C24" t="s">
+        <v>200</v>
+      </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1029,6 +1110,9 @@
       <c r="B25" t="s">
         <v>1</v>
       </c>
+      <c r="C25" t="s">
+        <v>200</v>
+      </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1038,6 +1122,9 @@
       <c r="B26" t="s">
         <v>197</v>
       </c>
+      <c r="C26" t="s">
+        <v>199</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1047,6 +1134,9 @@
       <c r="B27" t="s">
         <v>64</v>
       </c>
+      <c r="C27" t="s">
+        <v>199</v>
+      </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1056,6 +1146,9 @@
       <c r="B28" t="s">
         <v>37</v>
       </c>
+      <c r="C28" t="s">
+        <v>200</v>
+      </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1065,6 +1158,9 @@
       <c r="B29" t="s">
         <v>1</v>
       </c>
+      <c r="C29" t="s">
+        <v>199</v>
+      </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1074,6 +1170,9 @@
       <c r="B30" t="s">
         <v>14</v>
       </c>
+      <c r="C30" t="s">
+        <v>199</v>
+      </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1083,6 +1182,9 @@
       <c r="B31" t="s">
         <v>37</v>
       </c>
+      <c r="C31" t="s">
+        <v>200</v>
+      </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1092,6 +1194,9 @@
       <c r="B32" t="s">
         <v>10</v>
       </c>
+      <c r="C32" t="s">
+        <v>200</v>
+      </c>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1101,6 +1206,9 @@
       <c r="B33" t="s">
         <v>23</v>
       </c>
+      <c r="C33" t="s">
+        <v>200</v>
+      </c>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1110,6 +1218,9 @@
       <c r="B34" t="s">
         <v>14</v>
       </c>
+      <c r="C34" t="s">
+        <v>199</v>
+      </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1119,6 +1230,9 @@
       <c r="B35" t="s">
         <v>23</v>
       </c>
+      <c r="C35" t="s">
+        <v>200</v>
+      </c>
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1128,6 +1242,9 @@
       <c r="B36" t="s">
         <v>1</v>
       </c>
+      <c r="C36" t="s">
+        <v>199</v>
+      </c>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1137,6 +1254,9 @@
       <c r="B37" t="s">
         <v>3</v>
       </c>
+      <c r="C37" t="s">
+        <v>200</v>
+      </c>
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1146,6 +1266,9 @@
       <c r="B38" t="s">
         <v>19</v>
       </c>
+      <c r="C38" t="s">
+        <v>200</v>
+      </c>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1155,6 +1278,9 @@
       <c r="B39" t="s">
         <v>1</v>
       </c>
+      <c r="C39" t="s">
+        <v>199</v>
+      </c>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1164,6 +1290,9 @@
       <c r="B40" t="s">
         <v>1</v>
       </c>
+      <c r="C40" t="s">
+        <v>199</v>
+      </c>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1173,6 +1302,9 @@
       <c r="B41" t="s">
         <v>1</v>
       </c>
+      <c r="C41" t="s">
+        <v>199</v>
+      </c>
       <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1182,6 +1314,9 @@
       <c r="B42" t="s">
         <v>52</v>
       </c>
+      <c r="C42" t="s">
+        <v>200</v>
+      </c>
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1191,6 +1326,9 @@
       <c r="B43" t="s">
         <v>23</v>
       </c>
+      <c r="C43" t="s">
+        <v>199</v>
+      </c>
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1200,6 +1338,9 @@
       <c r="B44" t="s">
         <v>64</v>
       </c>
+      <c r="C44" t="s">
+        <v>200</v>
+      </c>
       <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1209,6 +1350,9 @@
       <c r="B45" t="s">
         <v>23</v>
       </c>
+      <c r="C45" t="s">
+        <v>199</v>
+      </c>
       <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1218,6 +1362,9 @@
       <c r="B46" t="s">
         <v>196</v>
       </c>
+      <c r="C46" t="s">
+        <v>200</v>
+      </c>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1227,6 +1374,9 @@
       <c r="B47" t="s">
         <v>19</v>
       </c>
+      <c r="C47" t="s">
+        <v>200</v>
+      </c>
       <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1236,6 +1386,9 @@
       <c r="B48" t="s">
         <v>1</v>
       </c>
+      <c r="C48" t="s">
+        <v>199</v>
+      </c>
       <c r="D48" s="1"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1245,6 +1398,9 @@
       <c r="B49" t="s">
         <v>5</v>
       </c>
+      <c r="C49" t="s">
+        <v>199</v>
+      </c>
       <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1254,6 +1410,9 @@
       <c r="B50" t="s">
         <v>23</v>
       </c>
+      <c r="C50" t="s">
+        <v>200</v>
+      </c>
       <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1263,6 +1422,9 @@
       <c r="B51" t="s">
         <v>8</v>
       </c>
+      <c r="C51" t="s">
+        <v>200</v>
+      </c>
       <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1272,6 +1434,9 @@
       <c r="B52" t="s">
         <v>23</v>
       </c>
+      <c r="C52" t="s">
+        <v>199</v>
+      </c>
       <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1281,6 +1446,9 @@
       <c r="B53" t="s">
         <v>64</v>
       </c>
+      <c r="C53" t="s">
+        <v>199</v>
+      </c>
       <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1290,6 +1458,9 @@
       <c r="B54" t="s">
         <v>5</v>
       </c>
+      <c r="C54" t="s">
+        <v>199</v>
+      </c>
       <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1299,6 +1470,9 @@
       <c r="B55" t="s">
         <v>14</v>
       </c>
+      <c r="C55" t="s">
+        <v>199</v>
+      </c>
       <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1308,6 +1482,9 @@
       <c r="B56" t="s">
         <v>14</v>
       </c>
+      <c r="C56" t="s">
+        <v>199</v>
+      </c>
       <c r="D56" s="1"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1317,6 +1494,9 @@
       <c r="B57" t="s">
         <v>1</v>
       </c>
+      <c r="C57" t="s">
+        <v>199</v>
+      </c>
       <c r="D57" s="1"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1326,6 +1506,9 @@
       <c r="B58" t="s">
         <v>14</v>
       </c>
+      <c r="C58" t="s">
+        <v>199</v>
+      </c>
       <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1335,6 +1518,9 @@
       <c r="B59" t="s">
         <v>197</v>
       </c>
+      <c r="C59" t="s">
+        <v>199</v>
+      </c>
       <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1344,6 +1530,9 @@
       <c r="B60" t="s">
         <v>8</v>
       </c>
+      <c r="C60" t="s">
+        <v>200</v>
+      </c>
       <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1353,6 +1542,9 @@
       <c r="B61" t="s">
         <v>3</v>
       </c>
+      <c r="C61" t="s">
+        <v>200</v>
+      </c>
       <c r="D61" s="1"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1362,6 +1554,9 @@
       <c r="B62" t="s">
         <v>3</v>
       </c>
+      <c r="C62" t="s">
+        <v>200</v>
+      </c>
       <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1371,6 +1566,9 @@
       <c r="B63" t="s">
         <v>5</v>
       </c>
+      <c r="C63" t="s">
+        <v>200</v>
+      </c>
       <c r="D63" s="1"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1378,7 +1576,10 @@
         <v>75</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>200</v>
       </c>
       <c r="D64" s="1"/>
     </row>
@@ -1387,7 +1588,10 @@
         <v>76</v>
       </c>
       <c r="B65" t="s">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="C65" t="s">
+        <v>199</v>
       </c>
       <c r="D65" s="1"/>
     </row>
@@ -1398,6 +1602,9 @@
       <c r="B66" t="s">
         <v>1</v>
       </c>
+      <c r="C66" t="s">
+        <v>200</v>
+      </c>
       <c r="D66" s="1"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1407,6 +1614,9 @@
       <c r="B67" t="s">
         <v>23</v>
       </c>
+      <c r="C67" t="s">
+        <v>199</v>
+      </c>
       <c r="D67" s="1"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1416,6 +1626,9 @@
       <c r="B68" t="s">
         <v>64</v>
       </c>
+      <c r="C68" t="s">
+        <v>199</v>
+      </c>
       <c r="D68" s="1"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1425,6 +1638,9 @@
       <c r="B69" t="s">
         <v>1</v>
       </c>
+      <c r="C69" t="s">
+        <v>199</v>
+      </c>
       <c r="D69" s="1"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -1434,6 +1650,9 @@
       <c r="B70" t="s">
         <v>14</v>
       </c>
+      <c r="C70" t="s">
+        <v>199</v>
+      </c>
       <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -1443,6 +1662,9 @@
       <c r="B71" t="s">
         <v>3</v>
       </c>
+      <c r="C71" t="s">
+        <v>200</v>
+      </c>
       <c r="D71" s="1"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1452,6 +1674,9 @@
       <c r="B72" t="s">
         <v>23</v>
       </c>
+      <c r="C72" t="s">
+        <v>199</v>
+      </c>
       <c r="D72" s="1"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1461,6 +1686,9 @@
       <c r="B73" t="s">
         <v>8</v>
       </c>
+      <c r="C73" t="s">
+        <v>199</v>
+      </c>
       <c r="D73" s="1"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1470,6 +1698,9 @@
       <c r="B74" t="s">
         <v>23</v>
       </c>
+      <c r="C74" t="s">
+        <v>200</v>
+      </c>
       <c r="D74" s="1"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -1479,6 +1710,9 @@
       <c r="B75" t="s">
         <v>3</v>
       </c>
+      <c r="C75" t="s">
+        <v>200</v>
+      </c>
       <c r="D75" s="1"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -1488,6 +1722,9 @@
       <c r="B76" t="s">
         <v>14</v>
       </c>
+      <c r="C76" t="s">
+        <v>199</v>
+      </c>
       <c r="D76" s="1"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -1497,6 +1734,9 @@
       <c r="B77" t="s">
         <v>8</v>
       </c>
+      <c r="C77" t="s">
+        <v>200</v>
+      </c>
       <c r="D77" s="1"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -1506,6 +1746,9 @@
       <c r="B78" t="s">
         <v>19</v>
       </c>
+      <c r="C78" t="s">
+        <v>200</v>
+      </c>
       <c r="D78" s="1"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -1515,6 +1758,9 @@
       <c r="B79" t="s">
         <v>31</v>
       </c>
+      <c r="C79" t="s">
+        <v>200</v>
+      </c>
       <c r="D79" s="1"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -1524,6 +1770,9 @@
       <c r="B80" t="s">
         <v>3</v>
       </c>
+      <c r="C80" t="s">
+        <v>200</v>
+      </c>
       <c r="D80" s="1"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -1533,6 +1782,9 @@
       <c r="B81" t="s">
         <v>93</v>
       </c>
+      <c r="C81" t="s">
+        <v>200</v>
+      </c>
       <c r="D81" s="1"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -1542,6 +1794,9 @@
       <c r="B82" t="s">
         <v>23</v>
       </c>
+      <c r="C82" t="s">
+        <v>199</v>
+      </c>
       <c r="D82" s="1"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -1551,6 +1806,9 @@
       <c r="B83" t="s">
         <v>19</v>
       </c>
+      <c r="C83" t="s">
+        <v>200</v>
+      </c>
       <c r="D83" s="1"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -1560,6 +1818,9 @@
       <c r="B84" t="s">
         <v>8</v>
       </c>
+      <c r="C84" t="s">
+        <v>200</v>
+      </c>
       <c r="D84" s="1"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -1569,6 +1830,9 @@
       <c r="B85" t="s">
         <v>14</v>
       </c>
+      <c r="C85" t="s">
+        <v>199</v>
+      </c>
       <c r="D85" s="1"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -1578,6 +1842,9 @@
       <c r="B86" t="s">
         <v>1</v>
       </c>
+      <c r="C86" t="s">
+        <v>200</v>
+      </c>
       <c r="D86" s="1"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -1587,6 +1854,9 @@
       <c r="B87" t="s">
         <v>8</v>
       </c>
+      <c r="C87" t="s">
+        <v>200</v>
+      </c>
       <c r="D87" s="1"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -1596,6 +1866,9 @@
       <c r="B88" t="s">
         <v>3</v>
       </c>
+      <c r="C88" t="s">
+        <v>199</v>
+      </c>
       <c r="D88" s="1"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -1605,6 +1878,9 @@
       <c r="B89" t="s">
         <v>8</v>
       </c>
+      <c r="C89" t="s">
+        <v>200</v>
+      </c>
       <c r="D89" s="1"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -1614,6 +1890,9 @@
       <c r="B90" t="s">
         <v>1</v>
       </c>
+      <c r="C90" t="s">
+        <v>199</v>
+      </c>
       <c r="D90" s="1"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -1623,6 +1902,9 @@
       <c r="B91" t="s">
         <v>8</v>
       </c>
+      <c r="C91" t="s">
+        <v>199</v>
+      </c>
       <c r="D91" s="1"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -1632,6 +1914,9 @@
       <c r="B92" t="s">
         <v>19</v>
       </c>
+      <c r="C92" t="s">
+        <v>200</v>
+      </c>
       <c r="D92" s="1"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -1641,6 +1926,9 @@
       <c r="B93" t="s">
         <v>23</v>
       </c>
+      <c r="C93" t="s">
+        <v>200</v>
+      </c>
       <c r="D93" s="1"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -1650,6 +1938,9 @@
       <c r="B94" t="s">
         <v>14</v>
       </c>
+      <c r="C94" t="s">
+        <v>199</v>
+      </c>
       <c r="D94" s="1"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -1659,6 +1950,9 @@
       <c r="B95" t="s">
         <v>23</v>
       </c>
+      <c r="C95" t="s">
+        <v>199</v>
+      </c>
       <c r="D95" s="1"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -1668,6 +1962,9 @@
       <c r="B96" t="s">
         <v>23</v>
       </c>
+      <c r="C96" t="s">
+        <v>200</v>
+      </c>
       <c r="D96" s="1"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -1677,6 +1974,9 @@
       <c r="B97" t="s">
         <v>1</v>
       </c>
+      <c r="C97" t="s">
+        <v>199</v>
+      </c>
       <c r="D97" s="1"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -1686,6 +1986,9 @@
       <c r="B98" t="s">
         <v>3</v>
       </c>
+      <c r="C98" t="s">
+        <v>200</v>
+      </c>
       <c r="D98" s="1"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -1695,6 +1998,9 @@
       <c r="B99" t="s">
         <v>1</v>
       </c>
+      <c r="C99" t="s">
+        <v>199</v>
+      </c>
       <c r="D99" s="1"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -1704,6 +2010,9 @@
       <c r="B100" t="s">
         <v>112</v>
       </c>
+      <c r="C100" t="s">
+        <v>199</v>
+      </c>
       <c r="D100" s="1"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -1713,6 +2022,9 @@
       <c r="B101" t="s">
         <v>64</v>
       </c>
+      <c r="C101" t="s">
+        <v>199</v>
+      </c>
       <c r="D101" s="1"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -1722,6 +2034,9 @@
       <c r="B102" t="s">
         <v>8</v>
       </c>
+      <c r="C102" t="s">
+        <v>199</v>
+      </c>
       <c r="D102" s="1"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -1731,6 +2046,9 @@
       <c r="B103" t="s">
         <v>3</v>
       </c>
+      <c r="C103" t="s">
+        <v>199</v>
+      </c>
       <c r="D103" s="1"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -1740,6 +2058,9 @@
       <c r="B104" t="s">
         <v>1</v>
       </c>
+      <c r="C104" t="s">
+        <v>199</v>
+      </c>
       <c r="D104" s="1"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -1749,6 +2070,9 @@
       <c r="B105" t="s">
         <v>8</v>
       </c>
+      <c r="C105" t="s">
+        <v>200</v>
+      </c>
       <c r="D105" s="1"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -1758,6 +2082,9 @@
       <c r="B106" t="s">
         <v>23</v>
       </c>
+      <c r="C106" t="s">
+        <v>199</v>
+      </c>
       <c r="D106" s="1"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -1767,6 +2094,9 @@
       <c r="B107" t="s">
         <v>23</v>
       </c>
+      <c r="C107" t="s">
+        <v>199</v>
+      </c>
       <c r="D107" s="1"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -1776,6 +2106,9 @@
       <c r="B108" t="s">
         <v>8</v>
       </c>
+      <c r="C108" t="s">
+        <v>199</v>
+      </c>
       <c r="D108" s="1"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -1785,6 +2118,9 @@
       <c r="B109" t="s">
         <v>8</v>
       </c>
+      <c r="C109" t="s">
+        <v>200</v>
+      </c>
       <c r="D109" s="1"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -1794,6 +2130,9 @@
       <c r="B110" t="s">
         <v>1</v>
       </c>
+      <c r="C110" t="s">
+        <v>199</v>
+      </c>
       <c r="D110" s="1"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -1803,6 +2142,9 @@
       <c r="B111" t="s">
         <v>124</v>
       </c>
+      <c r="C111" t="s">
+        <v>199</v>
+      </c>
       <c r="D111" s="1"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -1812,6 +2154,9 @@
       <c r="B112" t="s">
         <v>1</v>
       </c>
+      <c r="C112" t="s">
+        <v>199</v>
+      </c>
       <c r="D112" s="1"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -1821,6 +2166,9 @@
       <c r="B113" t="s">
         <v>5</v>
       </c>
+      <c r="C113" t="s">
+        <v>200</v>
+      </c>
       <c r="D113" s="1"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -1830,6 +2178,9 @@
       <c r="B114" t="s">
         <v>3</v>
       </c>
+      <c r="C114" t="s">
+        <v>200</v>
+      </c>
       <c r="D114" s="1"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -1839,6 +2190,9 @@
       <c r="B115" t="s">
         <v>14</v>
       </c>
+      <c r="C115" t="s">
+        <v>199</v>
+      </c>
       <c r="D115" s="1"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -1848,6 +2202,9 @@
       <c r="B116" t="s">
         <v>23</v>
       </c>
+      <c r="C116" t="s">
+        <v>200</v>
+      </c>
       <c r="D116" s="1"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -1857,6 +2214,9 @@
       <c r="B117" t="s">
         <v>16</v>
       </c>
+      <c r="C117" t="s">
+        <v>199</v>
+      </c>
       <c r="D117" s="1"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -1866,6 +2226,9 @@
       <c r="B118" t="s">
         <v>16</v>
       </c>
+      <c r="C118" t="s">
+        <v>200</v>
+      </c>
       <c r="D118" s="1"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -1875,6 +2238,9 @@
       <c r="B119" t="s">
         <v>1</v>
       </c>
+      <c r="C119" t="s">
+        <v>199</v>
+      </c>
       <c r="D119" s="1"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -1884,6 +2250,9 @@
       <c r="B120" t="s">
         <v>10</v>
       </c>
+      <c r="C120" t="s">
+        <v>199</v>
+      </c>
       <c r="D120" s="1"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -1893,6 +2262,9 @@
       <c r="B121" t="s">
         <v>31</v>
       </c>
+      <c r="C121" t="s">
+        <v>199</v>
+      </c>
       <c r="D121" s="1"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -1902,6 +2274,9 @@
       <c r="B122" t="s">
         <v>23</v>
       </c>
+      <c r="C122" t="s">
+        <v>199</v>
+      </c>
       <c r="D122" s="1"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -1911,6 +2286,9 @@
       <c r="B123" t="s">
         <v>1</v>
       </c>
+      <c r="C123" t="s">
+        <v>200</v>
+      </c>
       <c r="D123" s="1"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -1920,6 +2298,9 @@
       <c r="B124" t="s">
         <v>1</v>
       </c>
+      <c r="C124" t="s">
+        <v>199</v>
+      </c>
       <c r="D124" s="1"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -1929,6 +2310,9 @@
       <c r="B125" t="s">
         <v>14</v>
       </c>
+      <c r="C125" t="s">
+        <v>199</v>
+      </c>
       <c r="D125" s="1"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -1938,6 +2322,9 @@
       <c r="B126" t="s">
         <v>23</v>
       </c>
+      <c r="C126" t="s">
+        <v>199</v>
+      </c>
       <c r="D126" s="1"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -1947,6 +2334,9 @@
       <c r="B127" t="s">
         <v>141</v>
       </c>
+      <c r="C127" t="s">
+        <v>199</v>
+      </c>
       <c r="D127" s="1"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -1956,6 +2346,9 @@
       <c r="B128" t="s">
         <v>8</v>
       </c>
+      <c r="C128" t="s">
+        <v>200</v>
+      </c>
       <c r="D128" s="1"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -1965,6 +2358,9 @@
       <c r="B129" t="s">
         <v>8</v>
       </c>
+      <c r="C129" t="s">
+        <v>200</v>
+      </c>
       <c r="D129" s="1"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -1974,6 +2370,9 @@
       <c r="B130" t="s">
         <v>145</v>
       </c>
+      <c r="C130" t="s">
+        <v>200</v>
+      </c>
       <c r="D130" s="1"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -1983,6 +2382,9 @@
       <c r="B131" t="s">
         <v>3</v>
       </c>
+      <c r="C131" t="s">
+        <v>200</v>
+      </c>
       <c r="D131" s="1"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -1992,6 +2394,9 @@
       <c r="B132" t="s">
         <v>3</v>
       </c>
+      <c r="C132" t="s">
+        <v>200</v>
+      </c>
       <c r="D132" s="1"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -2001,6 +2406,9 @@
       <c r="B133" t="s">
         <v>31</v>
       </c>
+      <c r="C133" t="s">
+        <v>199</v>
+      </c>
       <c r="D133" s="1"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -2010,6 +2418,9 @@
       <c r="B134" t="s">
         <v>3</v>
       </c>
+      <c r="C134" t="s">
+        <v>200</v>
+      </c>
       <c r="D134" s="1"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -2019,6 +2430,9 @@
       <c r="B135" t="s">
         <v>152</v>
       </c>
+      <c r="C135" t="s">
+        <v>199</v>
+      </c>
       <c r="D135" s="1"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -2028,6 +2442,9 @@
       <c r="B136" t="s">
         <v>8</v>
       </c>
+      <c r="C136" t="s">
+        <v>199</v>
+      </c>
       <c r="D136" s="1"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -2037,6 +2454,9 @@
       <c r="B137" t="s">
         <v>64</v>
       </c>
+      <c r="C137" t="s">
+        <v>200</v>
+      </c>
       <c r="D137" s="1"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -2046,6 +2466,9 @@
       <c r="B138" t="s">
         <v>8</v>
       </c>
+      <c r="C138" t="s">
+        <v>199</v>
+      </c>
       <c r="D138" s="1"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -2055,6 +2478,9 @@
       <c r="B139" t="s">
         <v>157</v>
       </c>
+      <c r="C139" t="s">
+        <v>199</v>
+      </c>
       <c r="D139" s="1"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -2064,6 +2490,9 @@
       <c r="B140" t="s">
         <v>64</v>
       </c>
+      <c r="C140" t="s">
+        <v>199</v>
+      </c>
       <c r="D140" s="1"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -2073,6 +2502,9 @@
       <c r="B141" t="s">
         <v>1</v>
       </c>
+      <c r="C141" t="s">
+        <v>199</v>
+      </c>
       <c r="D141" s="1"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -2082,6 +2514,9 @@
       <c r="B142" t="s">
         <v>3</v>
       </c>
+      <c r="C142" t="s">
+        <v>200</v>
+      </c>
       <c r="D142" s="1"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -2091,6 +2526,9 @@
       <c r="B143" t="s">
         <v>14</v>
       </c>
+      <c r="C143" t="s">
+        <v>199</v>
+      </c>
       <c r="D143" s="1"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -2100,6 +2538,9 @@
       <c r="B144" t="s">
         <v>64</v>
       </c>
+      <c r="C144" t="s">
+        <v>199</v>
+      </c>
       <c r="D144" s="1"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -2109,6 +2550,9 @@
       <c r="B145" t="s">
         <v>1</v>
       </c>
+      <c r="C145" t="s">
+        <v>199</v>
+      </c>
       <c r="D145" s="1"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -2118,6 +2562,9 @@
       <c r="B146" t="s">
         <v>14</v>
       </c>
+      <c r="C146" t="s">
+        <v>199</v>
+      </c>
       <c r="D146" s="1"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -2127,6 +2574,9 @@
       <c r="B147" t="s">
         <v>166</v>
       </c>
+      <c r="C147" t="s">
+        <v>199</v>
+      </c>
       <c r="D147" s="1"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -2136,6 +2586,9 @@
       <c r="B148" t="s">
         <v>3</v>
       </c>
+      <c r="C148" t="s">
+        <v>200</v>
+      </c>
       <c r="D148" s="1"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -2145,6 +2598,9 @@
       <c r="B149" t="s">
         <v>145</v>
       </c>
+      <c r="C149" t="s">
+        <v>200</v>
+      </c>
       <c r="D149" s="1"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -2154,6 +2610,9 @@
       <c r="B150" t="s">
         <v>3</v>
       </c>
+      <c r="C150" t="s">
+        <v>200</v>
+      </c>
       <c r="D150" s="1"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
@@ -2163,6 +2622,9 @@
       <c r="B151" t="s">
         <v>23</v>
       </c>
+      <c r="C151" t="s">
+        <v>199</v>
+      </c>
       <c r="D151" s="1"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -2172,6 +2634,9 @@
       <c r="B152" t="s">
         <v>23</v>
       </c>
+      <c r="C152" t="s">
+        <v>199</v>
+      </c>
       <c r="D152" s="1"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -2181,6 +2646,9 @@
       <c r="B153" t="s">
         <v>3</v>
       </c>
+      <c r="C153" t="s">
+        <v>200</v>
+      </c>
       <c r="D153" s="1"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -2190,6 +2658,9 @@
       <c r="B154" t="s">
         <v>147</v>
       </c>
+      <c r="C154" t="s">
+        <v>200</v>
+      </c>
       <c r="D154" s="1"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -2199,6 +2670,9 @@
       <c r="B155" t="s">
         <v>64</v>
       </c>
+      <c r="C155" t="s">
+        <v>199</v>
+      </c>
       <c r="D155" s="1"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -2208,6 +2682,9 @@
       <c r="B156" t="s">
         <v>124</v>
       </c>
+      <c r="C156" t="s">
+        <v>199</v>
+      </c>
       <c r="D156" s="1"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -2217,6 +2694,9 @@
       <c r="B157" t="s">
         <v>124</v>
       </c>
+      <c r="C157" t="s">
+        <v>199</v>
+      </c>
       <c r="D157" s="1"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -2226,6 +2706,9 @@
       <c r="B158" t="s">
         <v>14</v>
       </c>
+      <c r="C158" t="s">
+        <v>199</v>
+      </c>
       <c r="D158" s="1"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -2235,6 +2718,9 @@
       <c r="B159" t="s">
         <v>19</v>
       </c>
+      <c r="C159" t="s">
+        <v>200</v>
+      </c>
       <c r="D159" s="1"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -2244,6 +2730,9 @@
       <c r="B160" t="s">
         <v>124</v>
       </c>
+      <c r="C160" t="s">
+        <v>199</v>
+      </c>
       <c r="D160" s="1"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -2253,6 +2742,9 @@
       <c r="B161" t="s">
         <v>181</v>
       </c>
+      <c r="C161" t="s">
+        <v>199</v>
+      </c>
       <c r="D161" s="1"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -2262,6 +2754,9 @@
       <c r="B162" t="s">
         <v>5</v>
       </c>
+      <c r="C162" t="s">
+        <v>199</v>
+      </c>
       <c r="D162" s="1"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -2271,6 +2766,9 @@
       <c r="B163" t="s">
         <v>1</v>
       </c>
+      <c r="C163" t="s">
+        <v>199</v>
+      </c>
       <c r="D163" s="1"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -2280,6 +2778,9 @@
       <c r="B164" t="s">
         <v>8</v>
       </c>
+      <c r="C164" t="s">
+        <v>200</v>
+      </c>
       <c r="D164" s="1"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -2289,6 +2790,9 @@
       <c r="B165" t="s">
         <v>124</v>
       </c>
+      <c r="C165" t="s">
+        <v>200</v>
+      </c>
       <c r="D165" s="1"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -2298,6 +2802,9 @@
       <c r="B166" t="s">
         <v>3</v>
       </c>
+      <c r="C166" t="s">
+        <v>199</v>
+      </c>
       <c r="D166" s="1"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -2307,6 +2814,9 @@
       <c r="B167" t="s">
         <v>14</v>
       </c>
+      <c r="C167" t="s">
+        <v>199</v>
+      </c>
       <c r="D167" s="1"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -2316,6 +2826,9 @@
       <c r="B168" t="s">
         <v>157</v>
       </c>
+      <c r="C168" t="s">
+        <v>200</v>
+      </c>
       <c r="D168" s="1"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -2325,6 +2838,9 @@
       <c r="B169" t="s">
         <v>8</v>
       </c>
+      <c r="C169" t="s">
+        <v>200</v>
+      </c>
       <c r="D169" s="2"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
@@ -2334,6 +2850,9 @@
       <c r="B170" t="s">
         <v>19</v>
       </c>
+      <c r="C170" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
@@ -2341,6 +2860,9 @@
       </c>
       <c r="B171" t="s">
         <v>10</v>
+      </c>
+      <c r="C171" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>